<commit_message>
add cols to 'raw' data that need to be added in order to agree with master
</commit_message>
<xml_diff>
--- a/inst/extdata/mysid/Armys20.xlsx
+++ b/inst/extdata/mysid/Armys20.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanamies-galonski/Code/nrp/nrp/inst/extdata/mysid/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9187AC43-432C-AB4D-8E58-366BD691AEE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="324" yWindow="105" windowWidth="12272" windowHeight="6812"/>
+    <workbookView xWindow="3700" yWindow="2340" windowWidth="24220" windowHeight="17620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="88">
   <si>
     <t>FileName</t>
   </si>
@@ -212,16 +218,82 @@
   </si>
   <si>
     <t>M7214090.csv</t>
+  </si>
+  <si>
+    <t>DepthCat</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Deep</t>
+  </si>
+  <si>
+    <t>FWCP</t>
+  </si>
+  <si>
+    <t>KWS</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>FundingSource</t>
+  </si>
+  <si>
+    <t>FieldCollection</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>MonthCat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1009]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,6 +305,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -255,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -271,6 +356,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -280,6 +366,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -328,7 +417,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,9 +450,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -396,6 +502,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -571,22 +694,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AZ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.2" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,136 +723,151 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AF1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AL1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AO1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AP1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="4"/>
-      <c r="AW1" s="4"/>
-      <c r="AX1" s="4"/>
+      <c r="AW1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>46</v>
       </c>
@@ -742,134 +880,149 @@
       <c r="D2">
         <v>4</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2">
         <v>20</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>1905</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>222</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" t="s">
         <v>47</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
       <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
         <v>125</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>17</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>46</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
       <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
         <v>53</v>
       </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
         <v>7</v>
       </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
       <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
         <v>435.04244762854455</v>
       </c>
-      <c r="X2">
+      <c r="Z2">
         <v>3.2920223213148958</v>
       </c>
-      <c r="Y2">
+      <c r="AA2">
         <v>151.37832522171422</v>
       </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
       <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
         <v>197.30737548910466</v>
       </c>
-      <c r="AC2">
+      <c r="AE2">
         <v>8.7584027426931623</v>
       </c>
-      <c r="AD2">
+      <c r="AF2">
         <v>66.697008871866871</v>
       </c>
-      <c r="AE2">
-        <v>0</v>
-      </c>
-      <c r="AF2">
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
         <v>7.6093129818507146</v>
       </c>
-      <c r="AG2">
+      <c r="AI2">
         <v>0.56306306306306297</v>
       </c>
-      <c r="AH2">
+      <c r="AJ2">
         <v>7.6576576576576572E-2</v>
       </c>
-      <c r="AI2">
+      <c r="AK2">
         <v>0.2072072072072072</v>
       </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <v>0</v>
-      </c>
       <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
         <v>0.23873873873873874</v>
       </c>
-      <c r="AM2">
+      <c r="AO2">
         <v>4.5045045045045045E-3</v>
       </c>
-      <c r="AN2">
+      <c r="AP2">
         <v>3.1531531531531529E-2</v>
       </c>
-      <c r="AO2">
-        <v>0</v>
-      </c>
-      <c r="AP2">
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
         <v>4.5045045045045045E-3</v>
       </c>
-      <c r="AQ2">
-        <v>0</v>
-      </c>
-      <c r="AR2">
-        <v>0</v>
-      </c>
       <c r="AS2">
         <v>0</v>
       </c>
       <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
         <v>0.88888888888888884</v>
       </c>
+      <c r="AW2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -882,123 +1035,123 @@
       <c r="D3">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3">
         <v>20</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>1923</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>222</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" t="s">
         <v>49</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
       <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>123</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>28</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>46</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
       <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
         <v>34</v>
       </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
         <v>13</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <v>2</v>
       </c>
-      <c r="V3">
-        <v>0</v>
-      </c>
-      <c r="W3">
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
         <v>438.70961144840311</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <v>5.3495080318832677</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>165.4456151163989</v>
       </c>
-      <c r="Z3">
-        <v>0</v>
-      </c>
-      <c r="AA3">
-        <v>0</v>
-      </c>
       <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
         <v>122.08232711807243</v>
       </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
         <v>125.10180439700578</v>
       </c>
-      <c r="AE3">
+      <c r="AG3">
         <v>20.73035678504278</v>
       </c>
-      <c r="AF3">
-        <v>0</v>
-      </c>
-      <c r="AG3">
+      <c r="AH3">
+        <v>0</v>
+      </c>
+      <c r="AI3">
         <v>0.55405405405405406</v>
       </c>
-      <c r="AH3">
+      <c r="AJ3">
         <v>0.12612612612612611</v>
       </c>
-      <c r="AI3">
+      <c r="AK3">
         <v>0.2072072072072072</v>
       </c>
-      <c r="AJ3">
-        <v>0</v>
-      </c>
-      <c r="AK3">
-        <v>0</v>
-      </c>
       <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>0</v>
+      </c>
+      <c r="AN3">
         <v>0.15315315315315314</v>
       </c>
-      <c r="AM3">
-        <v>0</v>
-      </c>
-      <c r="AN3">
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
         <v>5.8558558558558557E-2</v>
       </c>
-      <c r="AO3">
+      <c r="AQ3">
         <v>9.0090090090090089E-3</v>
       </c>
-      <c r="AP3">
-        <v>0</v>
-      </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
       <c r="AR3">
         <v>0</v>
       </c>
@@ -1006,10 +1159,25 @@
         <v>0</v>
       </c>
       <c r="AT3">
+        <v>0</v>
+      </c>
+      <c r="AU3">
+        <v>0</v>
+      </c>
+      <c r="AV3">
         <v>0.8666666666666667</v>
       </c>
+      <c r="AW3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1022,134 +1190,149 @@
       <c r="D4">
         <v>4</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4">
         <v>20</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>2</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
       <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
         <v>2011</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>280</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" t="s">
         <v>47</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
       <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>178</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>22</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>78</v>
       </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
       <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
         <v>52</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>10</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>6</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <v>8</v>
       </c>
-      <c r="V4">
+      <c r="X4">
         <v>2</v>
       </c>
-      <c r="W4">
+      <c r="Y4">
         <v>692.39823104389711</v>
       </c>
-      <c r="X4">
+      <c r="Z4">
         <v>3.8019995249474903</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>226.19625040457333</v>
       </c>
-      <c r="Z4">
-        <v>0</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
       <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
         <v>195.30511578868447</v>
       </c>
-      <c r="AC4">
+      <c r="AE4">
         <v>98.327480665356063</v>
       </c>
-      <c r="AD4">
+      <c r="AF4">
         <v>62.286712391983784</v>
       </c>
-      <c r="AE4">
+      <c r="AG4">
         <v>91.592937627409469</v>
       </c>
-      <c r="AF4">
+      <c r="AH4">
         <v>14.887734640942464</v>
       </c>
-      <c r="AG4">
+      <c r="AI4">
         <v>0.63571428571428579</v>
       </c>
-      <c r="AH4">
+      <c r="AJ4">
         <v>7.857142857142857E-2</v>
       </c>
-      <c r="AI4">
+      <c r="AK4">
         <v>0.27857142857142858</v>
       </c>
-      <c r="AJ4">
-        <v>0</v>
-      </c>
-      <c r="AK4">
-        <v>0</v>
-      </c>
       <c r="AL4">
+        <v>0</v>
+      </c>
+      <c r="AM4">
+        <v>0</v>
+      </c>
+      <c r="AN4">
         <v>0.18571428571428572</v>
       </c>
-      <c r="AM4">
+      <c r="AO4">
         <v>3.5714285714285712E-2</v>
       </c>
-      <c r="AN4">
+      <c r="AP4">
         <v>2.1428571428571429E-2</v>
       </c>
-      <c r="AO4">
+      <c r="AQ4">
         <v>2.8571428571428571E-2</v>
       </c>
-      <c r="AP4">
+      <c r="AR4">
         <v>7.1428571428571426E-3</v>
       </c>
-      <c r="AQ4">
-        <v>0</v>
-      </c>
-      <c r="AR4">
-        <v>0</v>
-      </c>
       <c r="AS4">
         <v>0</v>
       </c>
       <c r="AT4">
+        <v>0</v>
+      </c>
+      <c r="AU4">
+        <v>0</v>
+      </c>
+      <c r="AV4">
         <v>0.30769230769230771</v>
       </c>
+      <c r="AW4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY4" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -1162,120 +1345,120 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5">
         <v>20</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
         <v>2041</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>277</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" t="s">
         <v>49</v>
       </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
       <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
         <v>330</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>100</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>116</v>
       </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
       <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
         <v>94</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>2</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>18</v>
       </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
       <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
         <v>984.21388669359328</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
         <v>17.21923398875051</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>336.75900798365285</v>
       </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5">
-        <v>0</v>
-      </c>
       <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
         <v>437.11652738592466</v>
       </c>
-      <c r="AC5">
+      <c r="AE5">
         <v>23.046222255549349</v>
       </c>
-      <c r="AD5">
+      <c r="AF5">
         <v>170.07289507971601</v>
       </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
-      <c r="AF5">
-        <v>0</v>
-      </c>
       <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
         <v>1.1913357400722022</v>
       </c>
-      <c r="AH5">
+      <c r="AJ5">
         <v>0.36101083032490977</v>
       </c>
-      <c r="AI5">
+      <c r="AK5">
         <v>0.41877256317689532</v>
       </c>
-      <c r="AJ5">
-        <v>0</v>
-      </c>
-      <c r="AK5">
-        <v>0</v>
-      </c>
       <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>0</v>
+      </c>
+      <c r="AN5">
         <v>0.33935018050541516</v>
       </c>
-      <c r="AM5">
+      <c r="AO5">
         <v>7.2202166064981952E-3</v>
       </c>
-      <c r="AN5">
+      <c r="AP5">
         <v>6.4981949458483748E-2</v>
       </c>
-      <c r="AO5">
-        <v>0</v>
-      </c>
-      <c r="AP5">
-        <v>0</v>
-      </c>
       <c r="AQ5">
         <v>0</v>
       </c>
@@ -1286,10 +1469,25 @@
         <v>0</v>
       </c>
       <c r="AT5">
+        <v>0</v>
+      </c>
+      <c r="AU5">
+        <v>0</v>
+      </c>
+      <c r="AV5">
         <v>0.9</v>
       </c>
+      <c r="AW5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY5" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1302,134 +1500,149 @@
       <c r="D6">
         <v>4</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6">
         <v>20</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>3</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
       <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>2140</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>183</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" t="s">
         <v>47</v>
       </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
       <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
         <v>148</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>44</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>49</v>
       </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
       <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
         <v>36</v>
       </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
         <v>16</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <v>2</v>
       </c>
-      <c r="V6">
-        <v>1</v>
-      </c>
-      <c r="W6">
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
         <v>481.64249687310701</v>
       </c>
-      <c r="X6">
+      <c r="Z6">
         <v>8.6765852470013218</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>173.07414995601366</v>
       </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
       <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
         <v>110.98401927150167</v>
       </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
         <v>161.57177794954171</v>
       </c>
-      <c r="AE6">
+      <c r="AG6">
         <v>17.76038840730298</v>
       </c>
-      <c r="AF6">
+      <c r="AH6">
         <v>9.575576041745677</v>
       </c>
-      <c r="AG6">
+      <c r="AI6">
         <v>0.80874316939890711</v>
       </c>
-      <c r="AH6">
+      <c r="AJ6">
         <v>0.24043715846994534</v>
       </c>
-      <c r="AI6">
+      <c r="AK6">
         <v>0.26775956284153007</v>
       </c>
-      <c r="AJ6">
-        <v>0</v>
-      </c>
-      <c r="AK6">
-        <v>0</v>
-      </c>
       <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
         <v>0.19672131147540983</v>
       </c>
-      <c r="AM6">
-        <v>0</v>
-      </c>
-      <c r="AN6">
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
         <v>8.7431693989071038E-2</v>
       </c>
-      <c r="AO6">
+      <c r="AQ6">
         <v>1.092896174863388E-2</v>
       </c>
-      <c r="AP6">
+      <c r="AR6">
         <v>5.4644808743169399E-3</v>
       </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
-      <c r="AR6">
-        <v>0</v>
-      </c>
       <c r="AS6">
         <v>0</v>
       </c>
       <c r="AT6">
+        <v>0</v>
+      </c>
+      <c r="AU6">
+        <v>0</v>
+      </c>
+      <c r="AV6">
         <v>0.89473684210526316</v>
       </c>
+      <c r="AW6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY6" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -1442,134 +1655,149 @@
       <c r="D7">
         <v>4</v>
       </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7">
         <v>20</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>3</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>2200</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>179</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" t="s">
         <v>49</v>
       </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
       <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
         <v>146</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>36</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>39</v>
       </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
       <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
         <v>45</v>
       </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
         <v>21</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <v>3</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <v>2</v>
       </c>
-      <c r="W7">
+      <c r="Y7">
         <v>523.23772473873964</v>
       </c>
-      <c r="X7">
+      <c r="Z7">
         <v>6.527322561801137</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <v>125.34190675501461</v>
       </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7">
-        <v>0</v>
-      </c>
       <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
         <v>147.77231270197268</v>
       </c>
-      <c r="AC7">
-        <v>0</v>
-      </c>
-      <c r="AD7">
+      <c r="AE7">
+        <v>0</v>
+      </c>
+      <c r="AF7">
         <v>193.84868885997096</v>
       </c>
-      <c r="AE7">
+      <c r="AG7">
         <v>28.901858915404166</v>
       </c>
-      <c r="AF7">
+      <c r="AH7">
         <v>20.845634944576187</v>
       </c>
-      <c r="AG7">
+      <c r="AI7">
         <v>0.81564245810055869</v>
       </c>
-      <c r="AH7">
+      <c r="AJ7">
         <v>0.2011173184357542</v>
       </c>
-      <c r="AI7">
+      <c r="AK7">
         <v>0.21787709497206703</v>
       </c>
-      <c r="AJ7">
-        <v>0</v>
-      </c>
-      <c r="AK7">
-        <v>0</v>
-      </c>
       <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>0</v>
+      </c>
+      <c r="AN7">
         <v>0.25139664804469275</v>
       </c>
-      <c r="AM7">
-        <v>0</v>
-      </c>
-      <c r="AN7">
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
         <v>0.11731843575418995</v>
       </c>
-      <c r="AO7">
+      <c r="AQ7">
         <v>1.6759776536312849E-2</v>
       </c>
-      <c r="AP7">
+      <c r="AR7">
         <v>1.11731843575419E-2</v>
       </c>
-      <c r="AQ7">
-        <v>0</v>
-      </c>
-      <c r="AR7">
-        <v>0</v>
-      </c>
       <c r="AS7">
         <v>0</v>
       </c>
       <c r="AT7">
+        <v>0</v>
+      </c>
+      <c r="AU7">
+        <v>0</v>
+      </c>
+      <c r="AV7">
         <v>0.88461538461538458</v>
       </c>
+      <c r="AW7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY7" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -1582,123 +1810,123 @@
       <c r="D8">
         <v>4</v>
       </c>
-      <c r="E8">
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8">
         <v>22</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>6</v>
       </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
       <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>1850</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>158</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" t="s">
         <v>47</v>
       </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
-      </c>
       <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
         <v>132</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>47</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>42</v>
       </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
       <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
         <v>36</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>2</v>
       </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8">
+      <c r="V8">
+        <v>1</v>
+      </c>
+      <c r="W8">
         <v>4</v>
       </c>
-      <c r="V8">
-        <v>0</v>
-      </c>
-      <c r="W8">
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
         <v>498.52411781152074</v>
       </c>
-      <c r="X8">
+      <c r="Z8">
         <v>9.0869305653624739</v>
       </c>
-      <c r="Y8">
+      <c r="AA8">
         <v>194.74245873017412</v>
       </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8">
-        <v>0</v>
-      </c>
       <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
         <v>214.18103276883119</v>
       </c>
-      <c r="AC8">
+      <c r="AE8">
         <v>24.745851166793514</v>
       </c>
-      <c r="AD8">
+      <c r="AF8">
         <v>7.8381529123534825</v>
       </c>
-      <c r="AE8">
+      <c r="AG8">
         <v>47.92969166800593</v>
       </c>
-      <c r="AF8">
-        <v>0</v>
-      </c>
-      <c r="AG8">
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
         <v>0.83544303797468344</v>
       </c>
-      <c r="AH8">
+      <c r="AJ8">
         <v>0.29746835443037972</v>
       </c>
-      <c r="AI8">
+      <c r="AK8">
         <v>0.26582278481012656</v>
       </c>
-      <c r="AJ8">
-        <v>0</v>
-      </c>
-      <c r="AK8">
-        <v>0</v>
-      </c>
       <c r="AL8">
+        <v>0</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
         <v>0.22784810126582278</v>
       </c>
-      <c r="AM8">
+      <c r="AO8">
         <v>1.2658227848101266E-2</v>
       </c>
-      <c r="AN8">
+      <c r="AP8">
         <v>6.3291139240506328E-3</v>
       </c>
-      <c r="AO8">
+      <c r="AQ8">
         <v>2.5316455696202531E-2</v>
       </c>
-      <c r="AP8">
-        <v>0</v>
-      </c>
-      <c r="AQ8">
-        <v>0</v>
-      </c>
       <c r="AR8">
         <v>0</v>
       </c>
@@ -1706,10 +1934,25 @@
         <v>0</v>
       </c>
       <c r="AT8">
+        <v>0</v>
+      </c>
+      <c r="AU8">
+        <v>0</v>
+      </c>
+      <c r="AV8">
         <v>0.14285714285714285</v>
       </c>
+      <c r="AW8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY8" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1722,123 +1965,123 @@
       <c r="D9">
         <v>4</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9">
         <v>22</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>6</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>2</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>1915</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>157</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" t="s">
         <v>49</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
       <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
         <v>172</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>34</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>54</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>4</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
         <v>60</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>4</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>8</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <v>8</v>
       </c>
-      <c r="V9">
-        <v>0</v>
-      </c>
-      <c r="W9">
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
         <v>932.85162525407009</v>
       </c>
-      <c r="X9">
+      <c r="Z9">
         <v>6.9216487807743654</v>
       </c>
-      <c r="Y9">
+      <c r="AA9">
         <v>314.32867725657519</v>
       </c>
-      <c r="Z9">
+      <c r="AB9">
         <v>17.59378058089284</v>
       </c>
-      <c r="AA9">
-        <v>0</v>
-      </c>
-      <c r="AB9">
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
         <v>379.52350743514415</v>
       </c>
-      <c r="AC9">
+      <c r="AE9">
         <v>24.247842304924113</v>
       </c>
-      <c r="AD9">
+      <c r="AF9">
         <v>102.05682027925543</v>
       </c>
-      <c r="AE9">
+      <c r="AG9">
         <v>88.17934861650393</v>
       </c>
-      <c r="AF9">
-        <v>0</v>
-      </c>
-      <c r="AG9">
+      <c r="AH9">
+        <v>0</v>
+      </c>
+      <c r="AI9">
         <v>1.0955414012738853</v>
       </c>
-      <c r="AH9">
+      <c r="AJ9">
         <v>0.21656050955414013</v>
       </c>
-      <c r="AI9">
+      <c r="AK9">
         <v>0.34394904458598724</v>
       </c>
-      <c r="AJ9">
+      <c r="AL9">
         <v>2.5477707006369428E-2</v>
       </c>
-      <c r="AK9">
-        <v>0</v>
-      </c>
-      <c r="AL9">
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
         <v>0.38216560509554143</v>
       </c>
-      <c r="AM9">
+      <c r="AO9">
         <v>2.5477707006369428E-2</v>
       </c>
-      <c r="AN9">
+      <c r="AP9">
         <v>5.0955414012738856E-2</v>
       </c>
-      <c r="AO9">
+      <c r="AQ9">
         <v>5.0955414012738856E-2</v>
       </c>
-      <c r="AP9">
-        <v>0</v>
-      </c>
-      <c r="AQ9">
-        <v>0</v>
-      </c>
       <c r="AR9">
         <v>0</v>
       </c>
@@ -1846,10 +2089,25 @@
         <v>0</v>
       </c>
       <c r="AT9">
+        <v>0</v>
+      </c>
+      <c r="AU9">
+        <v>0</v>
+      </c>
+      <c r="AV9">
         <v>0.4</v>
       </c>
+      <c r="AW9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY9" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -1862,123 +2120,123 @@
       <c r="D10">
         <v>4</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10">
         <v>22</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>7</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
       <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
         <v>2005</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>139</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" t="s">
         <v>47</v>
       </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
       <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
         <v>53</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>10</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>18</v>
       </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
       <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
         <v>12</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>6</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>6</v>
       </c>
-      <c r="U10">
-        <v>1</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
       <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
         <v>306.11256637947196</v>
       </c>
-      <c r="X10">
+      <c r="Z10">
         <v>2.0243551521026633</v>
       </c>
-      <c r="Y10">
+      <c r="AA10">
         <v>91.841349100791007</v>
       </c>
-      <c r="Z10">
-        <v>0</v>
-      </c>
-      <c r="AA10">
-        <v>0</v>
-      </c>
       <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
         <v>63.596016238732759</v>
       </c>
-      <c r="AC10">
+      <c r="AE10">
         <v>63.582243045429436</v>
       </c>
-      <c r="AD10">
+      <c r="AF10">
         <v>74.067647718782851</v>
       </c>
-      <c r="AE10">
+      <c r="AG10">
         <v>11.000955123633297</v>
       </c>
-      <c r="AF10">
-        <v>0</v>
-      </c>
-      <c r="AG10">
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
         <v>0.38129496402877699</v>
       </c>
-      <c r="AH10">
+      <c r="AJ10">
         <v>7.1942446043165464E-2</v>
       </c>
-      <c r="AI10">
+      <c r="AK10">
         <v>0.12949640287769784</v>
       </c>
-      <c r="AJ10">
-        <v>0</v>
-      </c>
-      <c r="AK10">
-        <v>0</v>
-      </c>
       <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <v>0</v>
+      </c>
+      <c r="AN10">
         <v>8.6330935251798566E-2</v>
       </c>
-      <c r="AM10">
+      <c r="AO10">
         <v>4.3165467625899283E-2</v>
       </c>
-      <c r="AN10">
+      <c r="AP10">
         <v>4.3165467625899283E-2</v>
       </c>
-      <c r="AO10">
+      <c r="AQ10">
         <v>7.1942446043165471E-3</v>
       </c>
-      <c r="AP10">
-        <v>0</v>
-      </c>
-      <c r="AQ10">
-        <v>0</v>
-      </c>
       <c r="AR10">
         <v>0</v>
       </c>
@@ -1986,10 +2244,25 @@
         <v>0</v>
       </c>
       <c r="AT10">
+        <v>0</v>
+      </c>
+      <c r="AU10">
+        <v>0</v>
+      </c>
+      <c r="AV10">
         <v>0.46153846153846156</v>
       </c>
+      <c r="AW10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX10" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY10" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -2002,50 +2275,50 @@
       <c r="D11">
         <v>4</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11">
         <v>22</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>7</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>2</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>1949</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>141</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" t="s">
         <v>49</v>
       </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
       <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
         <v>58</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>14</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>18</v>
       </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
       <c r="R11">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="S11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T11">
         <v>12</v>
@@ -2054,58 +2327,58 @@
         <v>1</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
         <v>323.07224357526979</v>
       </c>
-      <c r="X11">
+      <c r="Z11">
         <v>2.5844687096886338</v>
       </c>
-      <c r="Y11">
+      <c r="AA11">
         <v>100.07771987807342</v>
       </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
       <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
         <v>75.925197992104174</v>
       </c>
-      <c r="AC11">
+      <c r="AE11">
         <v>7.4401345997774113</v>
       </c>
-      <c r="AD11">
+      <c r="AF11">
         <v>125.99644215449135</v>
       </c>
-      <c r="AE11">
+      <c r="AG11">
         <v>11.048280241134746</v>
       </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
         <v>0.41134751773049649</v>
       </c>
-      <c r="AH11">
+      <c r="AJ11">
         <v>9.9290780141843976E-2</v>
       </c>
-      <c r="AI11">
+      <c r="AK11">
         <v>0.1276595744680851</v>
       </c>
-      <c r="AJ11">
-        <v>0</v>
-      </c>
-      <c r="AK11">
-        <v>0</v>
-      </c>
       <c r="AL11">
-        <v>8.5106382978723402E-2</v>
+        <v>0</v>
       </c>
       <c r="AM11">
-        <v>7.0921985815602835E-3</v>
+        <v>0</v>
       </c>
       <c r="AN11">
         <v>8.5106382978723402E-2</v>
@@ -2114,10 +2387,10 @@
         <v>7.0921985815602835E-3</v>
       </c>
       <c r="AP11">
-        <v>0</v>
+        <v>8.5106382978723402E-2</v>
       </c>
       <c r="AQ11">
-        <v>0</v>
+        <v>7.0921985815602835E-3</v>
       </c>
       <c r="AR11">
         <v>0</v>
@@ -2126,10 +2399,25 @@
         <v>0</v>
       </c>
       <c r="AT11">
+        <v>0</v>
+      </c>
+      <c r="AU11">
+        <v>0</v>
+      </c>
+      <c r="AV11">
         <v>0.8571428571428571</v>
       </c>
+      <c r="AW11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -2142,120 +2430,120 @@
       <c r="D12">
         <v>4</v>
       </c>
-      <c r="E12">
+      <c r="E12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12">
         <v>22</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>8</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
       <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>2045</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>85</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" t="s">
         <v>47</v>
       </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
       <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
         <v>24</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>6</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>4</v>
       </c>
-      <c r="P12">
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
       <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
         <v>3</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>2</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>9</v>
       </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
       <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
         <v>169.56147699817555</v>
       </c>
-      <c r="X12">
+      <c r="Z12">
         <v>0.98650440978538056</v>
       </c>
-      <c r="Y12">
+      <c r="AA12">
         <v>20.750104522360562</v>
       </c>
-      <c r="Z12">
-        <v>0</v>
-      </c>
-      <c r="AA12">
-        <v>0</v>
-      </c>
       <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
         <v>19.501931060369742</v>
       </c>
-      <c r="AC12">
+      <c r="AE12">
         <v>22.373868802257569</v>
       </c>
-      <c r="AD12">
+      <c r="AF12">
         <v>105.94906820340231</v>
       </c>
-      <c r="AE12">
-        <v>0</v>
-      </c>
-      <c r="AF12">
-        <v>0</v>
-      </c>
       <c r="AG12">
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
         <v>0.28235294117647058</v>
       </c>
-      <c r="AH12">
+      <c r="AJ12">
         <v>7.0588235294117646E-2</v>
       </c>
-      <c r="AI12">
+      <c r="AK12">
         <v>4.7058823529411764E-2</v>
       </c>
-      <c r="AJ12">
-        <v>0</v>
-      </c>
-      <c r="AK12">
-        <v>0</v>
-      </c>
       <c r="AL12">
+        <v>0</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
         <v>3.5294117647058823E-2</v>
       </c>
-      <c r="AM12">
+      <c r="AO12">
         <v>2.3529411764705882E-2</v>
       </c>
-      <c r="AN12">
+      <c r="AP12">
         <v>0.10588235294117647</v>
       </c>
-      <c r="AO12">
-        <v>0</v>
-      </c>
-      <c r="AP12">
-        <v>0</v>
-      </c>
       <c r="AQ12">
         <v>0</v>
       </c>
@@ -2266,10 +2554,25 @@
         <v>0</v>
       </c>
       <c r="AT12">
+        <v>0</v>
+      </c>
+      <c r="AU12">
+        <v>0</v>
+      </c>
+      <c r="AV12">
         <v>0.81818181818181823</v>
       </c>
+      <c r="AW12" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY12" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -2282,122 +2585,122 @@
       <c r="D13">
         <v>4</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13">
         <v>22</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>8</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>2</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>2055</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>84</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" t="s">
         <v>49</v>
       </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
       <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
         <v>43</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>4</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>11</v>
       </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
       <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
         <v>10</v>
-      </c>
-      <c r="S13">
-        <v>2</v>
-      </c>
-      <c r="T13">
-        <v>14</v>
       </c>
       <c r="U13">
         <v>2</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="W13">
+        <v>2</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
         <v>364.50950397234948</v>
       </c>
-      <c r="X13">
+      <c r="Z13">
         <v>0.82767678336438322</v>
       </c>
-      <c r="Y13">
+      <c r="AA13">
         <v>79.285981478370118</v>
       </c>
-      <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AA13">
-        <v>0</v>
-      </c>
       <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
         <v>63.713703149583438</v>
       </c>
-      <c r="AC13">
+      <c r="AE13">
         <v>24.515705342582265</v>
       </c>
-      <c r="AD13">
+      <c r="AF13">
         <v>170.20751738964998</v>
       </c>
-      <c r="AE13">
+      <c r="AG13">
         <v>25.958919828799331</v>
       </c>
-      <c r="AF13">
-        <v>0</v>
-      </c>
-      <c r="AG13">
+      <c r="AH13">
+        <v>0</v>
+      </c>
+      <c r="AI13">
         <v>0.51190476190476186</v>
       </c>
-      <c r="AH13">
+      <c r="AJ13">
         <v>4.7619047619047616E-2</v>
       </c>
-      <c r="AI13">
+      <c r="AK13">
         <v>0.13095238095238096</v>
       </c>
-      <c r="AJ13">
-        <v>0</v>
-      </c>
-      <c r="AK13">
-        <v>0</v>
-      </c>
       <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13">
+        <v>0</v>
+      </c>
+      <c r="AN13">
         <v>0.11904761904761904</v>
-      </c>
-      <c r="AM13">
-        <v>2.3809523809523808E-2</v>
-      </c>
-      <c r="AN13">
-        <v>0.16666666666666666</v>
       </c>
       <c r="AO13">
         <v>2.3809523809523808E-2</v>
       </c>
       <c r="AP13">
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="AQ13">
-        <v>0</v>
+        <v>2.3809523809523808E-2</v>
       </c>
       <c r="AR13">
         <v>0</v>
@@ -2406,10 +2709,25 @@
         <v>0</v>
       </c>
       <c r="AT13">
+        <v>0</v>
+      </c>
+      <c r="AU13">
+        <v>0</v>
+      </c>
+      <c r="AV13">
         <v>0.77777777777777779</v>
       </c>
+      <c r="AW13" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX13" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY13" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -2422,134 +2740,149 @@
       <c r="D14">
         <v>5</v>
       </c>
-      <c r="E14">
+      <c r="E14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14">
         <v>19</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>7</v>
       </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
       <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
         <v>2000</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>160</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" t="s">
         <v>49</v>
       </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
       <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
         <v>151</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>114</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>13</v>
       </c>
-      <c r="P14">
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <v>0</v>
-      </c>
       <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
         <v>9</v>
       </c>
-      <c r="S14">
+      <c r="U14">
         <v>7</v>
       </c>
-      <c r="T14">
+      <c r="V14">
         <v>3</v>
       </c>
-      <c r="U14">
+      <c r="W14">
         <v>4</v>
       </c>
-      <c r="V14">
-        <v>1</v>
-      </c>
-      <c r="W14">
+      <c r="X14">
+        <v>1</v>
+      </c>
+      <c r="Y14">
         <v>402.85714823554724</v>
       </c>
-      <c r="X14">
+      <c r="Z14">
         <v>31.40360153783028</v>
       </c>
-      <c r="Y14">
+      <c r="AA14">
         <v>92.646237692969407</v>
       </c>
-      <c r="Z14">
-        <v>0</v>
-      </c>
-      <c r="AA14">
-        <v>0</v>
-      </c>
       <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
         <v>85.149107205702578</v>
       </c>
-      <c r="AC14">
+      <c r="AE14">
         <v>76.738666160379793</v>
       </c>
-      <c r="AD14">
+      <c r="AF14">
         <v>51.698030174961794</v>
       </c>
-      <c r="AE14">
+      <c r="AG14">
         <v>56.796381164072798</v>
       </c>
-      <c r="AF14">
+      <c r="AH14">
         <v>8.4251242996306441</v>
       </c>
-      <c r="AG14">
+      <c r="AI14">
         <v>0.94375000000000009</v>
       </c>
-      <c r="AH14">
+      <c r="AJ14">
         <v>0.71250000000000002</v>
       </c>
-      <c r="AI14">
+      <c r="AK14">
         <v>8.1250000000000003E-2</v>
       </c>
-      <c r="AJ14">
-        <v>0</v>
-      </c>
-      <c r="AK14">
-        <v>0</v>
-      </c>
       <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
         <v>5.6250000000000001E-2</v>
       </c>
-      <c r="AM14">
+      <c r="AO14">
         <v>4.3749999999999997E-2</v>
       </c>
-      <c r="AN14">
+      <c r="AP14">
         <v>1.8749999999999999E-2</v>
       </c>
-      <c r="AO14">
+      <c r="AQ14">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AP14">
+      <c r="AR14">
         <v>6.2500000000000003E-3</v>
       </c>
-      <c r="AQ14">
-        <v>0</v>
-      </c>
-      <c r="AR14">
-        <v>0</v>
-      </c>
       <c r="AS14">
         <v>0</v>
       </c>
       <c r="AT14">
+        <v>0</v>
+      </c>
+      <c r="AU14">
+        <v>0</v>
+      </c>
+      <c r="AV14">
         <v>0.26666666666666666</v>
       </c>
+      <c r="AW14" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX14" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY14" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -2562,123 +2895,123 @@
       <c r="D15">
         <v>5</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15">
         <v>19</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>7</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>2</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>2010</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>160</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" t="s">
         <v>47</v>
       </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
       <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
         <v>136</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>108</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>10</v>
       </c>
-      <c r="P15">
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
       <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
         <v>8</v>
       </c>
-      <c r="S15">
+      <c r="U15">
         <v>4</v>
       </c>
-      <c r="T15">
-        <v>1</v>
-      </c>
-      <c r="U15">
+      <c r="V15">
+        <v>1</v>
+      </c>
+      <c r="W15">
         <v>5</v>
       </c>
-      <c r="V15">
-        <v>0</v>
-      </c>
-      <c r="W15">
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
         <v>283.57514713775834</v>
       </c>
-      <c r="X15">
+      <c r="Z15">
         <v>27.840591130426979</v>
       </c>
-      <c r="Y15">
+      <c r="AA15">
         <v>67.198319263073586</v>
       </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AA15">
-        <v>0</v>
-      </c>
       <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
         <v>55.295538421547484</v>
       </c>
-      <c r="AC15">
+      <c r="AE15">
         <v>59.088990663058915</v>
       </c>
-      <c r="AD15">
+      <c r="AF15">
         <v>11.533828438632682</v>
       </c>
-      <c r="AE15">
+      <c r="AG15">
         <v>62.617879221018654</v>
       </c>
-      <c r="AF15">
-        <v>0</v>
-      </c>
-      <c r="AG15">
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
         <v>0.85000000000000009</v>
       </c>
-      <c r="AH15">
+      <c r="AJ15">
         <v>0.67500000000000004</v>
       </c>
-      <c r="AI15">
+      <c r="AK15">
         <v>6.25E-2</v>
       </c>
-      <c r="AJ15">
-        <v>0</v>
-      </c>
-      <c r="AK15">
-        <v>0</v>
-      </c>
       <c r="AL15">
+        <v>0</v>
+      </c>
+      <c r="AM15">
+        <v>0</v>
+      </c>
+      <c r="AN15">
         <v>0.05</v>
       </c>
-      <c r="AM15">
+      <c r="AO15">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AN15">
+      <c r="AP15">
         <v>6.2500000000000003E-3</v>
       </c>
-      <c r="AO15">
+      <c r="AQ15">
         <v>3.125E-2</v>
       </c>
-      <c r="AP15">
-        <v>0</v>
-      </c>
-      <c r="AQ15">
-        <v>0</v>
-      </c>
       <c r="AR15">
         <v>0</v>
       </c>
@@ -2686,10 +3019,25 @@
         <v>0</v>
       </c>
       <c r="AT15">
+        <v>0</v>
+      </c>
+      <c r="AU15">
+        <v>0</v>
+      </c>
+      <c r="AV15">
         <v>0.1</v>
       </c>
+      <c r="AW15" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX15" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY15" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>62</v>
       </c>
@@ -2702,117 +3050,117 @@
       <c r="D17">
         <v>7</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17">
         <v>14</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>7</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
       <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <v>2020</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>165</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" t="s">
         <v>49</v>
       </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
-      </c>
       <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
         <v>128</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <v>113</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>4</v>
       </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <v>0</v>
-      </c>
       <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
         <v>4</v>
       </c>
-      <c r="S17">
+      <c r="U17">
         <v>7</v>
       </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
       <c r="V17">
         <v>0</v>
       </c>
       <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
         <v>239.40385286159619</v>
       </c>
-      <c r="X17">
+      <c r="Z17">
         <v>78.665857372365579</v>
       </c>
-      <c r="Y17">
+      <c r="AA17">
         <v>34.931904693396206</v>
       </c>
-      <c r="Z17">
-        <v>0</v>
-      </c>
-      <c r="AA17">
-        <v>0</v>
-      </c>
       <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
         <v>42.548879609282935</v>
       </c>
-      <c r="AC17">
+      <c r="AE17">
         <v>83.257211186551473</v>
       </c>
-      <c r="AD17">
-        <v>0</v>
-      </c>
-      <c r="AE17">
-        <v>0</v>
-      </c>
       <c r="AF17">
         <v>0</v>
       </c>
       <c r="AG17">
+        <v>0</v>
+      </c>
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
         <v>0.77575757575757587</v>
       </c>
-      <c r="AH17">
+      <c r="AJ17">
         <v>0.68484848484848482</v>
       </c>
-      <c r="AI17">
+      <c r="AK17">
         <v>2.4242424242424242E-2</v>
       </c>
-      <c r="AJ17">
-        <v>0</v>
-      </c>
-      <c r="AK17">
-        <v>0</v>
-      </c>
       <c r="AL17">
+        <v>0</v>
+      </c>
+      <c r="AM17">
+        <v>0</v>
+      </c>
+      <c r="AN17">
         <v>2.4242424242424242E-2</v>
       </c>
-      <c r="AM17">
+      <c r="AO17">
         <v>4.2424242424242427E-2</v>
       </c>
-      <c r="AN17">
-        <v>0</v>
-      </c>
-      <c r="AO17">
-        <v>0</v>
-      </c>
       <c r="AP17">
         <v>0</v>
       </c>
@@ -2828,8 +3176,23 @@
       <c r="AT17">
         <v>0</v>
       </c>
+      <c r="AU17">
+        <v>0</v>
+      </c>
+      <c r="AV17">
+        <v>0</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -2842,117 +3205,117 @@
       <c r="D18">
         <v>7</v>
       </c>
-      <c r="E18">
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18">
         <v>14</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>7</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>2</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>2040</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>165</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" t="s">
         <v>47</v>
       </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
       <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
         <v>164</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <v>127</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>13</v>
       </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
       <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
         <v>11</v>
       </c>
-      <c r="S18">
+      <c r="U18">
         <v>13</v>
       </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
       <c r="V18">
         <v>0</v>
       </c>
       <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
         <v>392.3303755780712</v>
       </c>
-      <c r="X18">
+      <c r="Z18">
         <v>90.554658471491919</v>
       </c>
-      <c r="Y18">
+      <c r="AA18">
         <v>85.669402273054118</v>
       </c>
-      <c r="Z18">
-        <v>0</v>
-      </c>
-      <c r="AA18">
-        <v>0</v>
-      </c>
       <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
         <v>37.425676500898092</v>
       </c>
-      <c r="AC18">
+      <c r="AE18">
         <v>178.6806383326271</v>
       </c>
-      <c r="AD18">
-        <v>0</v>
-      </c>
-      <c r="AE18">
-        <v>0</v>
-      </c>
       <c r="AF18">
         <v>0</v>
       </c>
       <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
         <v>0.99393939393939379</v>
       </c>
-      <c r="AH18">
+      <c r="AJ18">
         <v>0.76969696969696966</v>
       </c>
-      <c r="AI18">
+      <c r="AK18">
         <v>7.8787878787878782E-2</v>
       </c>
-      <c r="AJ18">
-        <v>0</v>
-      </c>
-      <c r="AK18">
-        <v>0</v>
-      </c>
       <c r="AL18">
+        <v>0</v>
+      </c>
+      <c r="AM18">
+        <v>0</v>
+      </c>
+      <c r="AN18">
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="AM18">
+      <c r="AO18">
         <v>7.8787878787878782E-2</v>
       </c>
-      <c r="AN18">
-        <v>0</v>
-      </c>
-      <c r="AO18">
-        <v>0</v>
-      </c>
       <c r="AP18">
         <v>0</v>
       </c>
@@ -2968,8 +3331,23 @@
       <c r="AT18">
         <v>0</v>
       </c>
+      <c r="AU18">
+        <v>0</v>
+      </c>
+      <c r="AV18">
+        <v>0</v>
+      </c>
+      <c r="AW18" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX18" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY18" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -2982,117 +3360,117 @@
       <c r="D20">
         <v>9</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20">
         <v>14</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>7</v>
       </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
       <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <v>1900</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>167</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" t="s">
         <v>49</v>
       </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
       <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
         <v>186</v>
-      </c>
-      <c r="N20">
-        <v>20</v>
-      </c>
-      <c r="O20">
-        <v>50</v>
       </c>
       <c r="P20">
         <v>20</v>
       </c>
       <c r="Q20">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="R20">
+        <v>20</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
         <v>76</v>
       </c>
-      <c r="S20">
+      <c r="U20">
         <v>20</v>
       </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
       <c r="V20">
         <v>0</v>
       </c>
       <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
         <v>899.44130223235675</v>
       </c>
-      <c r="X20">
+      <c r="Z20">
         <v>11.416509335502239</v>
       </c>
-      <c r="Y20">
+      <c r="AA20">
         <v>161.578222602458</v>
       </c>
-      <c r="Z20">
+      <c r="AB20">
         <v>211.73276377875646</v>
       </c>
-      <c r="AA20">
-        <v>0</v>
-      </c>
-      <c r="AB20">
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
         <v>260.11661023348779</v>
       </c>
-      <c r="AC20">
+      <c r="AE20">
         <v>254.59719628215231</v>
       </c>
-      <c r="AD20">
-        <v>0</v>
-      </c>
-      <c r="AE20">
-        <v>0</v>
-      </c>
       <c r="AF20">
         <v>0</v>
       </c>
       <c r="AG20">
+        <v>0</v>
+      </c>
+      <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
         <v>1.1137724550898205</v>
-      </c>
-      <c r="AH20">
-        <v>0.11976047904191617</v>
-      </c>
-      <c r="AI20">
-        <v>0.29940119760479039</v>
       </c>
       <c r="AJ20">
         <v>0.11976047904191617</v>
       </c>
       <c r="AK20">
-        <v>0</v>
+        <v>0.29940119760479039</v>
       </c>
       <c r="AL20">
+        <v>0.11976047904191617</v>
+      </c>
+      <c r="AM20">
+        <v>0</v>
+      </c>
+      <c r="AN20">
         <v>0.45508982035928142</v>
       </c>
-      <c r="AM20">
+      <c r="AO20">
         <v>0.11976047904191617</v>
       </c>
-      <c r="AN20">
-        <v>0</v>
-      </c>
-      <c r="AO20">
-        <v>0</v>
-      </c>
       <c r="AP20">
         <v>0</v>
       </c>
@@ -3108,8 +3486,23 @@
       <c r="AT20">
         <v>0</v>
       </c>
+      <c r="AU20">
+        <v>0</v>
+      </c>
+      <c r="AV20">
+        <v>0</v>
+      </c>
+      <c r="AW20" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX20" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY20" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -3122,117 +3515,117 @@
       <c r="D21">
         <v>9</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F21">
         <v>14</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>7</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>2</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>1920</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <v>165</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" t="s">
         <v>47</v>
       </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
       <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
         <v>212</v>
       </c>
-      <c r="N21">
+      <c r="P21">
         <v>24</v>
       </c>
-      <c r="O21">
+      <c r="Q21">
         <v>79</v>
       </c>
-      <c r="P21">
+      <c r="R21">
         <v>10</v>
       </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
         <v>89</v>
       </c>
-      <c r="S21">
+      <c r="U21">
         <v>10</v>
       </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
       <c r="V21">
         <v>0</v>
       </c>
       <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
         <v>909.72530345402845</v>
       </c>
-      <c r="X21">
+      <c r="Z21">
         <v>18.392833172515843</v>
       </c>
-      <c r="Y21">
+      <c r="AA21">
         <v>323.69345906519078</v>
       </c>
-      <c r="Z21">
+      <c r="AB21">
         <v>106.2537540474685</v>
       </c>
-      <c r="AA21">
-        <v>0</v>
-      </c>
-      <c r="AB21">
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
         <v>338.9370351410447</v>
       </c>
-      <c r="AC21">
+      <c r="AE21">
         <v>122.44822202780855</v>
       </c>
-      <c r="AD21">
-        <v>0</v>
-      </c>
-      <c r="AE21">
-        <v>0</v>
-      </c>
       <c r="AF21">
         <v>0</v>
       </c>
       <c r="AG21">
+        <v>0</v>
+      </c>
+      <c r="AH21">
+        <v>0</v>
+      </c>
+      <c r="AI21">
         <v>1.2848484848484847</v>
       </c>
-      <c r="AH21">
+      <c r="AJ21">
         <v>0.14545454545454545</v>
       </c>
-      <c r="AI21">
+      <c r="AK21">
         <v>0.47878787878787876</v>
       </c>
-      <c r="AJ21">
+      <c r="AL21">
         <v>6.0606060606060608E-2</v>
       </c>
-      <c r="AK21">
-        <v>0</v>
-      </c>
-      <c r="AL21">
+      <c r="AM21">
+        <v>0</v>
+      </c>
+      <c r="AN21">
         <v>0.53939393939393943</v>
       </c>
-      <c r="AM21">
+      <c r="AO21">
         <v>6.0606060606060608E-2</v>
       </c>
-      <c r="AN21">
-        <v>0</v>
-      </c>
-      <c r="AO21">
-        <v>0</v>
-      </c>
       <c r="AP21">
         <v>0</v>
       </c>
@@ -3247,9 +3640,26 @@
       </c>
       <c r="AT21">
         <v>0</v>
+      </c>
+      <c r="AU21">
+        <v>0</v>
+      </c>
+      <c r="AV21">
+        <v>0</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX21" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY21" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>